<commit_message>
Updating PCA9685 Test code, correcting mistake in LV Buck converter spec, adding a rough sim for LV Buck
</commit_message>
<xml_diff>
--- a/Documentation/LV Buck Converter Calcs.xlsx
+++ b/Documentation/LV Buck Converter Calcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>LV Buck Converter Calculations</t>
   </si>
@@ -83,9 +83,6 @@
     <t>K-factor (0.2 &lt; x &lt; 0.4)</t>
   </si>
   <si>
-    <t>For LMR16006</t>
-  </si>
-  <si>
     <t>Datasheet</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Ceramic Cap ESR Insignificant, so calc ignored</t>
   </si>
   <si>
-    <t>2x 4.7u Ceramic Caps</t>
-  </si>
-  <si>
     <t>Diode Selection</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>100k // 100k</t>
   </si>
   <si>
-    <t>Murata LQH3NPN150MMEL</t>
-  </si>
-  <si>
     <t>Diodes Inc. MBR0580S1-7</t>
   </si>
   <si>
@@ -165,6 +156,39 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Capacitance (uF)</t>
+  </si>
+  <si>
+    <t>For LMR16006X</t>
+  </si>
+  <si>
+    <t>Max Load Step</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden NR4018T470M</t>
+  </si>
+  <si>
+    <t>In BOM</t>
+  </si>
+  <si>
+    <t>Cost:</t>
+  </si>
+  <si>
+    <t>(&lt;0.5%)</t>
+  </si>
+  <si>
+    <t>IC Selection</t>
+  </si>
+  <si>
+    <t>TI LM16006DDCR</t>
+  </si>
+  <si>
+    <t>&lt;- Accounting for DC Bias (actually 2x 1u + 100n)</t>
   </si>
 </sst>
 </file>
@@ -248,7 +272,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,6 +289,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -276,6 +303,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -559,42 +594,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="I1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -602,7 +632,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -611,17 +641,21 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8">
-        <v>5.71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8">
+        <f>SUM(J3:J1003)</f>
+        <v>5.1099999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
         <v>42</v>
@@ -630,347 +664,516 @@
         <v>30</v>
       </c>
       <c r="D3" s="2">
-        <f>B43</f>
+        <f>B46</f>
         <v>4.9729207920792078</v>
       </c>
       <c r="E3" s="2">
         <v>0.4</v>
       </c>
       <c r="F3" s="2">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="G3" s="2">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="16">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="J6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="J7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
+      <c r="J8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.78</v>
+      </c>
+      <c r="D9">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="F9" s="5">
+        <f>B15</f>
+        <v>0.47022916272336968</v>
+      </c>
+      <c r="G9" s="5">
+        <f>B13</f>
+        <v>0.3511458136168481</v>
+      </c>
+      <c r="J9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>D3+C9*D9</f>
+        <v>5.2864807920792076</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="16">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <f>(B11*(B3-B11))/(B3*B9*0.000001*H3*1000000)</f>
+        <v>0.14045832544673925</v>
+      </c>
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f>B12/E3</f>
+        <v>0.3511458136168481</v>
+      </c>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="D6">
-        <v>0.40200000000000002</v>
-      </c>
-      <c r="F6" s="5">
-        <f>B12</f>
-        <v>0.47127642090625838</v>
-      </c>
-      <c r="G6" s="5">
-        <f>B10</f>
-        <v>0.35638210453129177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <f>D3+C6*D6</f>
-        <v>5.112816792079208</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="B14">
+        <f>SQRT(E3^2 + B12^2/12)</f>
+        <v>0.40204980425183878</v>
+      </c>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f>E3+B12/2</f>
+        <v>0.47022916272336968</v>
+      </c>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
         <v>43</v>
       </c>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <f>(B8*(B3-B8))/(B3*B6*0.000001*G3*1000000)</f>
-        <v>0.14255284181251671</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <f>B9/E3</f>
-        <v>0.35638210453129177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <f>SQRT(E3^2 + B9^2/12)</f>
-        <v>0.40211123178261932</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <f>E3+B9/2</f>
-        <v>0.47127642090625838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C19" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="J19" s="16"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f>(2*F3)/(H3*1000000*G3)*1000000</f>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f>B9*0.000001*(E3^2)/((D3+G3)^2 - D3) * 1000000</f>
+        <v>0.36220707192535134</v>
+      </c>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>1/(8*H3*1000000) * B12/G3 * 1000000</f>
+        <v>0.25081843829774869</v>
+      </c>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
         <v>25</v>
       </c>
-      <c r="H15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <f>(2*E3)/(G3*1000000*F3)*1000000</f>
-        <v>7.6190476190476195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <f>B6*0.000001*(E3^2)/((D3+F3)^2 - D3) * 1000000</f>
-        <v>0.11847866000715869</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <f>1/(8*G3*1000000) * B9/F3 * 1000000</f>
-        <v>0.16970576406251986</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
         <f>B3*1.25</f>
         <v>52.5</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C29" s="4">
         <f>E3</f>
         <v>0.4</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="G29" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="16">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <f>E3*SQRT(B11/C3*(C3-B11)/C3)</f>
+        <v>0.15240154248117269</v>
+      </c>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <f>E3*0.25/(B33*0.000001*H3*1000000)*1000</f>
+        <v>129.87012987012989</v>
+      </c>
+      <c r="C35" t="s">
+        <v>51</v>
+      </c>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="16">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31">
-        <f>E3*SQRT(B8/C3*(C3-B8)/C3)</f>
-        <v>0.15040307810857781</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <f>E3*0.25/(B30*0.000001*G3*1000000)*1000</f>
-        <v>47.619047619047628</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>9.09</v>
+      </c>
+      <c r="J43" s="16"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40">
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" t="s">
         <v>50</v>
       </c>
-      <c r="C40">
-        <v>9.09</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="J44" s="16">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="16"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
-      <c r="B43">
-        <f xml:space="preserve"> 0.765*(1+B40/C40)</f>
+      <c r="B46">
+        <f xml:space="preserve"> 0.765*(1+B43/C43)</f>
         <v>4.9729207920792078</v>
       </c>
+      <c r="J46" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="H1:I1"/>
+  <mergeCells count="11">
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A41:E41"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1"/>
-    <hyperlink ref="F8" r:id="rId2"/>
-    <hyperlink ref="F26" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="G29" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Failing at making a custom bootloader and testing VCP
</commit_message>
<xml_diff>
--- a/Documentation/LV Buck Converter Calcs.xlsx
+++ b/Documentation/LV Buck Converter Calcs.xlsx
@@ -143,12 +143,6 @@
     <t>R_bot (kOhm)</t>
   </si>
   <si>
-    <t>10k // 100k</t>
-  </si>
-  <si>
-    <t>100k // 100k</t>
-  </si>
-  <si>
     <t>Diodes Inc. MBR0580S1-7</t>
   </si>
   <si>
@@ -189,6 +183,12 @@
   </si>
   <si>
     <t>&lt;- Accounting for DC Bias (actually 2x 1u + 100n)</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>10k // 10k + 390R</t>
   </si>
 </sst>
 </file>
@@ -289,21 +289,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -311,6 +296,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,17 +612,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="I1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="I1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -641,7 +641,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
@@ -652,7 +652,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8">
         <f>SUM(J3:J1003)</f>
-        <v>5.1099999999999994</v>
+        <v>5.1499999999999995</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -665,7 +665,7 @@
       </c>
       <c r="D3" s="2">
         <f>B46</f>
-        <v>4.9729207920792078</v>
+        <v>5.0228849721706865</v>
       </c>
       <c r="E3" s="2">
         <v>0.4</v>
@@ -679,25 +679,25 @@
       <c r="H3" s="2">
         <v>0.7</v>
       </c>
-      <c r="J3" s="16"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="J4" s="16"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>19</v>
@@ -705,16 +705,16 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="16">
+      <c r="G5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="11">
         <v>2.88</v>
       </c>
     </row>
@@ -724,17 +724,17 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="J6" s="16"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="J7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -755,7 +755,7 @@
       <c r="G8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -769,16 +769,16 @@
       </c>
       <c r="F9" s="5">
         <f>B15</f>
-        <v>0.47022916272336968</v>
+        <v>0.47079644083447791</v>
       </c>
       <c r="G9" s="5">
         <f>B13</f>
-        <v>0.3511458136168481</v>
-      </c>
-      <c r="J9" s="16"/>
+        <v>0.35398220417238929</v>
+      </c>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J10" s="16"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -786,18 +786,18 @@
       </c>
       <c r="B11">
         <f>D3+C9*D9</f>
-        <v>5.2864807920792076</v>
+        <v>5.3364449721706864</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s">
         <v>48</v>
       </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="16">
+      <c r="J11" s="11">
         <v>0.45</v>
       </c>
     </row>
@@ -807,9 +807,9 @@
       </c>
       <c r="B12">
         <f>(B11*(B3-B11))/(B3*B9*0.000001*H3*1000000)</f>
-        <v>0.14045832544673925</v>
-      </c>
-      <c r="J12" s="16"/>
+        <v>0.14159288166895573</v>
+      </c>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -817,9 +817,9 @@
       </c>
       <c r="B13">
         <f>B12/E3</f>
-        <v>0.3511458136168481</v>
-      </c>
-      <c r="J13" s="16"/>
+        <v>0.35398220417238929</v>
+      </c>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -827,9 +827,9 @@
       </c>
       <c r="B14">
         <f>SQRT(E3^2 + B12^2/12)</f>
-        <v>0.40204980425183878</v>
-      </c>
-      <c r="J14" s="16"/>
+        <v>0.40208296657730969</v>
+      </c>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -837,43 +837,43 @@
       </c>
       <c r="B15">
         <f>E3+B12/2</f>
-        <v>0.47022916272336968</v>
-      </c>
-      <c r="J15" s="16"/>
+        <v>0.47079644083447791</v>
+      </c>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="16"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="J17" s="16"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>44</v>
+      <c r="B18" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="16">
+        <v>48</v>
+      </c>
+      <c r="J18" s="11">
         <v>0.26</v>
       </c>
     </row>
@@ -884,13 +884,13 @@
       <c r="C19" s="4">
         <v>4.7</v>
       </c>
-      <c r="J19" s="16"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="16"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -900,7 +900,7 @@
         <f>(2*F3)/(H3*1000000*G3)*1000000</f>
         <v>8.5714285714285712</v>
       </c>
-      <c r="J21" s="16"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -908,9 +908,9 @@
       </c>
       <c r="B22">
         <f>B9*0.000001*(E3^2)/((D3+G3)^2 - D3) * 1000000</f>
-        <v>0.36220707192535134</v>
-      </c>
-      <c r="J22" s="16"/>
+        <v>0.35436486504771408</v>
+      </c>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -918,33 +918,33 @@
       </c>
       <c r="B23">
         <f>1/(8*H3*1000000) * B12/G3 * 1000000</f>
-        <v>0.25081843829774869</v>
-      </c>
-      <c r="J23" s="16"/>
+        <v>0.25284443155170666</v>
+      </c>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J24" s="16"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="J25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J26" s="16"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="J27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -956,7 +956,7 @@
       <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="16"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
@@ -968,30 +968,30 @@
         <v>0.4</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" t="s">
         <v>41</v>
       </c>
-      <c r="H29" t="s">
-        <v>43</v>
-      </c>
       <c r="I29" t="s">
-        <v>50</v>
-      </c>
-      <c r="J29" s="16">
+        <v>48</v>
+      </c>
+      <c r="J29" s="11">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J30" s="16"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="J31" s="16"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1000,27 +1000,27 @@
       <c r="B32" t="s">
         <v>31</v>
       </c>
-      <c r="J32" s="16"/>
+      <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="C33" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I33" t="s">
-        <v>50</v>
-      </c>
-      <c r="J33" s="16">
+        <v>48</v>
+      </c>
+      <c r="J33" s="11">
         <v>1.06</v>
       </c>
     </row>
@@ -1030,9 +1030,9 @@
       </c>
       <c r="B34">
         <f>E3*SQRT(B11/C3*(C3-B11)/C3)</f>
-        <v>0.15240154248117269</v>
-      </c>
-      <c r="J34" s="16"/>
+        <v>0.152965183677922</v>
+      </c>
+      <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1043,22 +1043,22 @@
         <v>129.87012987012989</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="16"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="J37" s="16"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1067,37 +1067,37 @@
       <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="J38" s="16"/>
+      <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I39" t="s">
-        <v>50</v>
-      </c>
-      <c r="J39" s="16">
+        <v>48</v>
+      </c>
+      <c r="J39" s="11">
         <v>0.06</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="16"/>
+      <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="J41" s="16"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1109,39 +1109,39 @@
       <c r="C42" t="s">
         <v>38</v>
       </c>
-      <c r="J42" s="16"/>
+      <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C43">
-        <v>9.09</v>
-      </c>
-      <c r="J43" s="16"/>
+        <v>5.39</v>
+      </c>
+      <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="G44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I44" t="s">
-        <v>50</v>
-      </c>
-      <c r="J44" s="16">
-        <v>0.12</v>
+        <v>48</v>
+      </c>
+      <c r="J44" s="11">
+        <v>0.16</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J45" s="16"/>
+      <c r="J45" s="11"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1149,9 +1149,9 @@
       </c>
       <c r="B46">
         <f xml:space="preserve"> 0.765*(1+B43/C43)</f>
-        <v>4.9729207920792078</v>
-      </c>
-      <c r="J46" s="16"/>
+        <v>5.0228849721706865</v>
+      </c>
+      <c r="J46" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>